<commit_message>
Change schedule and corrected emailto link
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jens.klenke\Documents\GitHub\RuhrMetrics_Reading_Group\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/513dcd0917740ba2/RGS documents/Reading group/RuhrMetrics_Reading_Group/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD568582-431A-44B0-84EC-5582F8E2C930}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{BD568582-431A-44B0-84EC-5582F8E2C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A56C900-978D-4315-BFEC-6B7EE93884BD}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Files</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -111,12 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,96 +435,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7243CAAD-E342-4971-AD06-AB4BE82344F7}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="129.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="115.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45610</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45638</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45666</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45680</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="155.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="155.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45694</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45708</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new meeting and presentation
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/513dcd0917740ba2/RGS documents/Reading group/RuhrMetrics_Reading_Group/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jens Klenke\Documents\GitHub\RuhrMetrics_Reading_Group\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{BD568582-431A-44B0-84EC-5582F8E2C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75918218-1FE9-43C5-8CA2-F084C0B5641F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F8DA59-8FAF-42CA-8A2A-A6BDC5894BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -57,9 +57,6 @@
     <t>&lt;a href="paper/Bollerslev_ConditionallyHeteroskedasticTime.pdf" download="Bollerslev_ConditionallyHeteroskedasticTime.pdf"&gt;A Conditionally Heteroskedastic Time Series Model for Speculative Prices and Rates of Return&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href = "paper/Hill_Bayesian_Nonparametric_Modeling_for_Causal_Inference.pdf" donwload="Hill_Bayesian_Nonparametric_Modeling_for_Causal_Inference.pdf"&gt; Bayesian Nonparametric Modeling for Causal Inference&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Sven Pappert</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>5 pm</t>
+  </si>
+  <si>
+    <t>&lt;a href = "paper/Hill_Bayesian_Nonparametric_Modeling_for_Causal_Inference.pdf" download="Hill_Bayesian_Nonparametric_Modeling_for_Causal_Inference.pdf"&gt; Bayesian Nonparametric Modeling for Causal Inference&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = "presentation/causal_macro_reading_group_WS24.pdf" download="causal_macro_reading_group_WS24.pdf"&gt;&amp;copy;&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -145,7 +148,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,22 +447,22 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="115.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="115.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -468,15 +471,15 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45610</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -484,13 +487,16 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45638</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -499,12 +505,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45666</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -513,49 +519,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45680</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45694</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45708</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
     </row>

</xml_diff>

<commit_message>
Removed Btissame, corrected Simon's date and changed date format.
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/513dcd0917740ba2/RGS documents/Reading group/RuhrMetrics_Reading_Group/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{4B31BDE5-82FA-4906-BBD4-7389B58DD5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C44BB0CB-1FF2-4D45-A269-2D89E56F5ABD}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{4B31BDE5-82FA-4906-BBD4-7389B58DD5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A922F933-7A01-4A21-B5F3-53D655C3B1F9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
+    <workbookView xWindow="-828" yWindow="-14508" windowWidth="23256" windowHeight="13896" xr2:uid="{8BAD8284-06BE-4115-98CF-B1E188670130}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -45,9 +45,6 @@
     <t>5 pm</t>
   </si>
   <si>
-    <t>&lt;a href = "paper_new/Bootstraps_for_time_series.pdf" download="Bootstraps_for_time_series.pdf"&gt;  Bootstrap for time series&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Timo Puschmann</t>
   </si>
   <si>
@@ -57,28 +54,25 @@
     <t>Daria Ovsyannikova</t>
   </si>
   <si>
-    <t>&lt;a href = "paper_new/Asymptotic_inference_about_predictive_ability.pdf" download="Asymptotic_inference_about_predictive_ability.pdf"&gt;Asymptotic Inference about Predictive Ability&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href="paper_new/LASSO-driven_inference_in_time_and_space.pdf" download="LASSO-driven_inference_in_time_and_space.pdf"&gt;LASSO-driven inference in time and space &lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = "paper_new/Regression_diagnostics_meets_forecast_evaluation-conditional_calibration,_reliability_diagrams,_and_coefficient_of_determination.pdf" download="Regression_diagnostics_meets_forecast_evaluation-conditional_calibration,_reliability_diagrams,_and_coefficient_of_determination.pdf"&gt; Regression diagnostics meets forecast evaluation: conditional calibration, reliability diagrams and coefficient of determination&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = "paper_new/Inference_on_heterogeneous_treatment_effects_in_high‐dimensional_dynamic_panels.pdf" download="Inference_on_heterogeneous_treatment_effects_in_high‐dimensional_dynamic_panels.pdf"&gt; Inference on heterogeneous treatment effects in high-dimensional dynamic panels under weak dependence&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Eva Oeß &amp; Lennard Massmann</t>
   </si>
   <si>
-    <t>Btissame El Mahtout</t>
-  </si>
-  <si>
     <t>Simon Hirsch</t>
   </si>
   <si>
-    <t>A combination of two papers: &lt;a href = "paper_new/Regularization_Paths_for_Generalized_Linear_Models_via_Coordinate_Descent.pdf" download="Regularization_Paths_for_Generalized_Linear_Models_via_Coordinate_Descent.pdf"&gt; Regularization Paths for Generalized Linear Models via Coordinate Descent&lt;/a&gt; and &lt;a href = "paper_new/Pathwise_coordinate_optimization.pdf" download="Pathwise_coordinate_optimization.pdf"&gt;  Pathwise coordinate optimization&lt;/a&gt;</t>
+    <t>&lt;a href = "paper/Regression_diagnostics_meets_forecast_evaluation-conditional_calibration,_reliability_diagrams,_and_coefficient_of_determination.pdf" download="Regression_diagnostics_meets_forecast_evaluation-conditional_calibration,_reliability_diagrams,_and_coefficient_of_determination.pdf"&gt; Regression diagnostics meets forecast evaluation: conditional calibration, reliability diagrams and coefficient of determination&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = "paper/Inference_on_heterogeneous_treatment_effects_in_high‐dimensional_dynamic_panels.pdf" download="Inference_on_heterogeneous_treatment_effects_in_high‐dimensional_dynamic_panels.pdf"&gt; Inference on heterogeneous treatment effects in high-dimensional dynamic panels under weak dependence&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>A combination of two papers: &lt;a href = "paper/Regularization_Paths_for_Generalized_Linear_Models_via_Coordinate_Descent.pdf" download="Regularization_Paths_for_Generalized_Linear_Models_via_Coordinate_Descent.pdf"&gt; Regularization Paths for Generalized Linear Models via Coordinate Descent&lt;/a&gt; and &lt;a href = "paper/Pathwise_coordinate_optimization.pdf" download="Pathwise_coordinate_optimization.pdf"&gt;  Pathwise coordinate optimization&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="paper/LASSO-driven_inference_in_time_and_space.pdf" download="LASSO-driven_inference_in_time_and_space.pdf"&gt;LASSO-driven inference in time and space &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = "paper/Bootstraps_for_time_series.pdf" download="Bootstraps_for_time_series.pdf"&gt;  Bootstrap for time series&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -438,21 +432,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7243CAAD-E342-4971-AD06-AB4BE82344F7}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="115.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="115.6640625" customWidth="1"/>
     <col min="5" max="5" width="120" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45771</v>
       </c>
@@ -477,13 +471,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45785</v>
       </c>
@@ -491,13 +485,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45813</v>
       </c>
@@ -505,58 +499,44 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>45848</v>
+        <v>45862</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>45869</v>
+        <v>45890</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
+      <c r="C6" t="s">
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>45890</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>